<commit_message>
Added the csv_time_conversion file, which tries to clean the data
Signed-off-by: NoahHenriques <noah.henriq@gmail.com>
</commit_message>
<xml_diff>
--- a/HungerLevels.xlsx
+++ b/HungerLevels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahh/Documents/GitHub/Senior-Project-Modeling-Noah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13CAA750-E1BF-9A42-B40D-7F7EC9F5024C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A416B5AA-B3E9-4D4F-A11E-EE3EC63117BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{48CB7CAF-F4B6-E94E-B5B9-A446A3390F54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Hunger</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9/17/24</t>
   </si>
 </sst>
 </file>
@@ -80,8 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32136D3-98C9-7944-B403-281FCFA0F49D}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,6 +443,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45552</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>